<commit_message>
SVN (res) commit #2184 by scriswellwsf       misc ruleset &amp; UI mods toward next 2022 Alpha release
</commit_message>
<xml_diff>
--- a/RulesetDev/Rulesets/CA Res/Rules/T24R_CommunitySolar.xlsx
+++ b/RulesetDev/Rulesets/CA Res/Rules/T24R_CommunitySolar.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\svn-CEC\SF_CBECC-Res\trunk\RulesetDev\Rulesets\CA Res\Rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Res\trunk\RulesetDev\Rulesets\CA Res\Rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBAF668-01ED-44F1-A89B-B1BB5EE4D91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195953E6-5CC2-461D-B06A-1E7FA59A5ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5528" yWindow="1485" windowWidth="16102" windowHeight="11423" xr2:uid="{451AA6B4-8F74-4A09-9E06-84A86EFCFE8F}"/>
+    <workbookView xWindow="40080" yWindow="30" windowWidth="14385" windowHeight="13920" xr2:uid="{451AA6B4-8F74-4A09-9E06-84A86EFCFE8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,15 +23,41 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Scott Criswell</author>
+  </authors>
+  <commentList>
+    <comment ref="H25" authorId="0" shapeId="0" xr:uid="{A46280DE-4DF3-4A3C-9569-B866A40973DC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Copy of 2019 data for TEMPORARY use in 2022 analysis</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>kTDV</t>
   </si>
@@ -115,7 +141,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,13 +170,32 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -194,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -210,6 +255,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,22 +570,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EABD591-F703-4994-B9A0-1B58CC57ECFD}">
-  <dimension ref="A1:J27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EABD591-F703-4994-B9A0-1B58CC57ECFD}">
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.3984375" customWidth="1"/>
-    <col min="4" max="4" width="10.53125" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="3.265625" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -546,7 +593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -554,12 +601,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -570,7 +617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -580,12 +627,12 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -596,12 +643,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -609,12 +656,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -622,7 +669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -633,7 +680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -644,12 +691,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -658,7 +705,7 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -669,7 +716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -680,7 +727,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -691,7 +738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -702,22 +749,22 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>25</v>
       </c>
@@ -737,7 +784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C24" s="8">
         <v>2019</v>
       </c>
@@ -763,38 +810,65 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C25" s="8" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="8">
+        <v>2022</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1</v>
+      </c>
+      <c r="E25" s="9">
+        <v>-2011.8</v>
+      </c>
+      <c r="F25" s="10">
+        <v>-0.1108</v>
+      </c>
+      <c r="G25" s="10">
+        <v>-56263</v>
+      </c>
+      <c r="H25" s="10">
+        <v>-333.12</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E26" s="6">
         <v>0</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <v>0</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <v>0</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A26" s="5"/>
-      <c r="B26" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SVN (res) commit #2219 by scriswellwsf       ruleset mods updating Community Solar for 2022 analysis
</commit_message>
<xml_diff>
--- a/RulesetDev/Rulesets/CA Res/Rules/T24R_CommunitySolar.xlsx
+++ b/RulesetDev/Rulesets/CA Res/Rules/T24R_CommunitySolar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Res\trunk\RulesetDev\Rulesets\CA Res\Rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195953E6-5CC2-461D-B06A-1E7FA59A5ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50B9785-97D7-4465-BB59-C8C7585A5DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40080" yWindow="30" windowWidth="14385" windowHeight="13920" xr2:uid="{451AA6B4-8F74-4A09-9E06-84A86EFCFE8F}"/>
+    <workbookView xWindow="8940" yWindow="780" windowWidth="16695" windowHeight="13095" xr2:uid="{451AA6B4-8F74-4A09-9E06-84A86EFCFE8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,16 +39,27 @@
     <author>Scott Criswell</author>
   </authors>
   <commentList>
-    <comment ref="H25" authorId="0" shapeId="0" xr:uid="{A46280DE-4DF3-4A3C-9569-B866A40973DC}">
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{F612DA61-0DE4-49A5-AB6A-EEF8CE9F726B}">
       <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SAC 05/25/22:</t>
+        </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Copy of 2019 data for TEMPORARY use in 2022 analysis</t>
+          <t xml:space="preserve">
+still based on 2019 Elec Demand multipliers</t>
         </r>
       </text>
     </comment>
@@ -57,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>kTDV</t>
   </si>
@@ -135,13 +146,22 @@
   </si>
   <si>
     <t>CodeBase</t>
+  </si>
+  <si>
+    <t>SrcKBtu</t>
+  </si>
+  <si>
+    <t>05/25/22 - SAC - added newly calculated SMUD Community Solar results for use in 2022 analysis</t>
+  </si>
+  <si>
+    <t>kBtu of Source Energy (EDR1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,7 +201,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -239,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -255,8 +282,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,18 +599,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EABD591-F703-4994-B9A0-1B58CC57ECFD}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="3.28515625" customWidth="1"/>
+    <col min="8" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -611,26 +639,28 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -716,7 +746,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -727,7 +757,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -738,7 +768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -749,121 +779,144 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="1" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C24" s="8">
+      <c r="I24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="8">
         <v>2019</v>
-      </c>
-      <c r="D24" s="8">
-        <v>1</v>
-      </c>
-      <c r="E24" s="6">
-        <v>-2011.8</v>
-      </c>
-      <c r="F24">
-        <v>-0.1108</v>
-      </c>
-      <c r="G24">
-        <v>-56263</v>
-      </c>
-      <c r="H24">
-        <v>-333.12</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C25" s="8">
-        <v>2022</v>
       </c>
       <c r="D25" s="8">
         <v>1</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="6">
         <v>-2011.8</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25">
         <v>-0.1108</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25">
         <v>-56263</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25">
         <v>-333.12</v>
       </c>
-      <c r="I25" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C26" s="8" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="8">
+        <v>2022</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1</v>
+      </c>
+      <c r="E26" s="10">
+        <v>-2137.9</v>
+      </c>
+      <c r="F26" s="9">
+        <v>-0.16089999999999999</v>
+      </c>
+      <c r="G26" s="11">
+        <v>-47454</v>
+      </c>
+      <c r="H26" s="11">
+        <v>-99.150999999999996</v>
+      </c>
+      <c r="I26" s="11">
+        <v>-1609.6</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D27" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E27" s="6">
         <v>0</v>
       </c>
-      <c r="F26">
+      <c r="F27">
         <v>0</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>0</v>
       </c>
-      <c r="H26">
+      <c r="H27">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" t="s">
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SVN (res) commit #2227 by scriswellwsf       updates to electric demand multipliers for 2022 weather &amp; code (tic #1267)
</commit_message>
<xml_diff>
--- a/RulesetDev/Rulesets/CA Res/Rules/T24R_CommunitySolar.xlsx
+++ b/RulesetDev/Rulesets/CA Res/Rules/T24R_CommunitySolar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Res\trunk\RulesetDev\Rulesets\CA Res\Rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50B9785-97D7-4465-BB59-C8C7585A5DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7915DA3-B771-4AA9-B6C6-8FFA94AF34FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="780" windowWidth="16695" windowHeight="13095" xr2:uid="{451AA6B4-8F74-4A09-9E06-84A86EFCFE8F}"/>
+    <workbookView xWindow="285" yWindow="1320" windowWidth="16485" windowHeight="13485" xr2:uid="{451AA6B4-8F74-4A09-9E06-84A86EFCFE8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,42 +33,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Scott Criswell</author>
-  </authors>
-  <commentList>
-    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{F612DA61-0DE4-49A5-AB6A-EEF8CE9F726B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>SAC 05/25/22:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-still based on 2019 Elec Demand multipliers</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
   <si>
     <t>kTDV</t>
   </si>
@@ -155,13 +121,16 @@
   </si>
   <si>
     <t>kBtu of Source Energy (EDR1)</t>
+  </si>
+  <si>
+    <t>06/01/22 - SAC - updated 2022 look-up values w/ latest 2022 kW multipliers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,39 +159,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -266,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -282,7 +225,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -598,11 +540,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EABD591-F703-4994-B9A0-1B58CC57ECFD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EABD591-F703-4994-B9A0-1B58CC57ECFD}">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +584,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -684,6 +626,9 @@
       </c>
       <c r="B9" t="s">
         <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -864,19 +809,19 @@
       <c r="D26" s="8">
         <v>1</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="9">
         <v>-2137.9</v>
       </c>
-      <c r="F26" s="9">
-        <v>-0.16089999999999999</v>
-      </c>
-      <c r="G26" s="11">
+      <c r="F26" s="10">
+        <v>-1.23E-2</v>
+      </c>
+      <c r="G26" s="10">
         <v>-47454</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="10">
         <v>-99.150999999999996</v>
       </c>
-      <c r="I26" s="11">
+      <c r="I26" s="10">
         <v>-1609.6</v>
       </c>
       <c r="J26" s="8" t="s">
@@ -922,6 +867,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>